<commit_message>
Endret på barnehage ID
</commit_message>
<xml_diff>
--- a/oblig5-gruppe/barnehage/kgdata.xlsx
+++ b/oblig5-gruppe/barnehage/kgdata.xlsx
@@ -642,7 +642,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -661,7 +661,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -680,7 +680,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -699,7 +699,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -718,7 +718,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -737,7 +737,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -756,7 +756,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -775,7 +775,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -794,7 +794,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -813,7 +813,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -832,7 +832,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -851,7 +851,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -870,7 +870,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -889,7 +889,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -908,7 +908,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -927,7 +927,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -946,7 +946,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -965,7 +965,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -984,7 +984,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1003,7 +1003,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1041,7 +1041,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1060,7 +1060,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1079,7 +1079,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1098,7 +1098,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1117,7 +1117,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1136,7 +1136,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Laget statistikk.html fil og lagt til statistikk i menyen og la til routingen
</commit_message>
<xml_diff>
--- a/oblig5-gruppe/barnehage/kgdata.xlsx
+++ b/oblig5-gruppe/barnehage/kgdata.xlsx
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E2" t="n">
         <v>15</v>
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
@@ -555,10 +555,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -574,10 +574,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -593,10 +593,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
@@ -612,10 +612,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8">
@@ -631,10 +631,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9">
@@ -650,10 +650,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10">
@@ -669,10 +669,10 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>40</v>
+        <v>148</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11">
@@ -688,10 +688,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12">
@@ -707,10 +707,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
@@ -726,10 +726,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
@@ -745,10 +745,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15">
@@ -764,10 +764,10 @@
         </is>
       </c>
       <c r="D15" t="n">
+        <v>59</v>
+      </c>
+      <c r="E15" t="n">
         <v>40</v>
-      </c>
-      <c r="E15" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="16">
@@ -783,10 +783,10 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17">
@@ -802,10 +802,10 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18">
@@ -821,10 +821,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
@@ -840,10 +840,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20">
@@ -859,10 +859,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21">
@@ -881,7 +881,7 @@
         <v>40</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22">
@@ -897,10 +897,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>40</v>
+        <v>206</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23">
@@ -916,10 +916,10 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24">
@@ -935,10 +935,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25">
@@ -954,10 +954,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26">
@@ -973,10 +973,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27">
@@ -992,10 +992,10 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28">
@@ -1011,10 +1011,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29">
@@ -1030,10 +1030,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30">
@@ -1052,7 +1052,7 @@
         <v>40</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31">
@@ -1068,10 +1068,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32">
@@ -1087,10 +1087,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33">
@@ -1106,10 +1106,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34">
@@ -1125,10 +1125,10 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35">
@@ -1144,10 +1144,10 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Løst oppgave 4. Laget funksjon for å vise diagram, oppdatert routing og gjort endringer på statistikk.html for å fremvise grafen basert på gitt kommune.
</commit_message>
<xml_diff>
--- a/oblig5-gruppe/barnehage/kgdata.xlsx
+++ b/oblig5-gruppe/barnehage/kgdata.xlsx
@@ -11,6 +11,7 @@
     <sheet name="barnehage" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="barn" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="soknad" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="statistikk" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1265,4 +1266,75 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>kom</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>y15</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>y16</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>y17</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>y18</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>y19</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>y20</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>y21</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>y22</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>y23</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
nå burde det være ferdig
</commit_message>
<xml_diff>
--- a/oblig5-gruppe/barnehage/kgdata.xlsx
+++ b/oblig5-gruppe/barnehage/kgdata.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,6 +462,54 @@
         <is>
           <t>foresatt_pnr</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>erfan sarwari</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>eigemyrveien 27</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>93097239</v>
+      </c>
+      <c r="F2" t="n">
+        <v>30090578123</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Erfan sarwari</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>eigemyrveien 26</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>94086394</v>
+      </c>
+      <c r="F3" t="n">
+        <v>30090714256</v>
       </c>
     </row>
   </sheetData>
@@ -1162,7 +1210,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1180,6 +1228,17 @@
         <is>
           <t>barn_pnr</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>30090234152</v>
       </c>
     </row>
   </sheetData>
@@ -1193,7 +1252,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:M1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1261,6 +1320,53 @@
         <is>
           <t>brutto_inntekt</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>1, 2, 3, 4, 5</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2024-11-29</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>900000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gjort det mer tydelig hvilke kommune vi har valgt i opgaven vår, design endringer på html statistikk, søknad og barnehager
</commit_message>
<xml_diff>
--- a/oblig5-gruppe/barnehage/kgdata.xlsx
+++ b/oblig5-gruppe/barnehage/kgdata.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="B1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,54 +462,6 @@
         <is>
           <t>foresatt_pnr</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>erfan sarwari</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>eigemyrveien 27</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>93097239</v>
-      </c>
-      <c r="F2" t="n">
-        <v>30090578123</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Erfan sarwari</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>eigemyrveien 26</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>94086394</v>
-      </c>
-      <c r="F3" t="n">
-        <v>30090714256</v>
       </c>
     </row>
   </sheetData>
@@ -569,7 +521,7 @@
         <v>38</v>
       </c>
       <c r="E2" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -588,7 +540,7 @@
         <v>70</v>
       </c>
       <c r="E3" t="n">
-        <v>67</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -607,7 +559,7 @@
         <v>83</v>
       </c>
       <c r="E4" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -626,7 +578,7 @@
         <v>61</v>
       </c>
       <c r="E5" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -645,7 +597,7 @@
         <v>54</v>
       </c>
       <c r="E6" t="n">
-        <v>50</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
@@ -664,7 +616,7 @@
         <v>74</v>
       </c>
       <c r="E7" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -683,7 +635,7 @@
         <v>92</v>
       </c>
       <c r="E8" t="n">
-        <v>78</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
@@ -702,7 +654,7 @@
         <v>53</v>
       </c>
       <c r="E9" t="n">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
@@ -721,7 +673,7 @@
         <v>148</v>
       </c>
       <c r="E10" t="n">
-        <v>138</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11">
@@ -740,7 +692,7 @@
         <v>98</v>
       </c>
       <c r="E11" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -759,7 +711,7 @@
         <v>47</v>
       </c>
       <c r="E12" t="n">
-        <v>46</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -778,7 +730,7 @@
         <v>73</v>
       </c>
       <c r="E13" t="n">
-        <v>60</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -797,7 +749,7 @@
         <v>60</v>
       </c>
       <c r="E14" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -816,7 +768,7 @@
         <v>59</v>
       </c>
       <c r="E15" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -835,7 +787,7 @@
         <v>66</v>
       </c>
       <c r="E16" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -854,7 +806,7 @@
         <v>35</v>
       </c>
       <c r="E17" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -873,7 +825,7 @@
         <v>82</v>
       </c>
       <c r="E18" t="n">
-        <v>80</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19">
@@ -892,7 +844,7 @@
         <v>96</v>
       </c>
       <c r="E19" t="n">
-        <v>66</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -911,7 +863,7 @@
         <v>51</v>
       </c>
       <c r="E20" t="n">
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
@@ -930,7 +882,7 @@
         <v>40</v>
       </c>
       <c r="E21" t="n">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
@@ -949,7 +901,7 @@
         <v>206</v>
       </c>
       <c r="E22" t="n">
-        <v>196</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23">
@@ -968,7 +920,7 @@
         <v>83</v>
       </c>
       <c r="E23" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -987,7 +939,7 @@
         <v>50</v>
       </c>
       <c r="E24" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
@@ -1006,7 +958,7 @@
         <v>61</v>
       </c>
       <c r="E25" t="n">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
@@ -1025,7 +977,7 @@
         <v>31</v>
       </c>
       <c r="E26" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -1044,7 +996,7 @@
         <v>43</v>
       </c>
       <c r="E27" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -1063,7 +1015,7 @@
         <v>59</v>
       </c>
       <c r="E28" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1082,7 +1034,7 @@
         <v>64</v>
       </c>
       <c r="E29" t="n">
-        <v>56</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30">
@@ -1101,7 +1053,7 @@
         <v>40</v>
       </c>
       <c r="E30" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -1139,7 +1091,7 @@
         <v>72</v>
       </c>
       <c r="E32" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1158,7 +1110,7 @@
         <v>51</v>
       </c>
       <c r="E33" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1177,7 +1129,7 @@
         <v>71</v>
       </c>
       <c r="E34" t="n">
-        <v>46</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -1196,7 +1148,7 @@
         <v>67</v>
       </c>
       <c r="E35" t="n">
-        <v>56</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1210,7 +1162,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="B1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1228,17 +1180,6 @@
         <is>
           <t>barn_pnr</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>30090234152</v>
       </c>
     </row>
   </sheetData>
@@ -1252,7 +1193,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="B1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1320,53 +1261,6 @@
         <is>
           <t>brutto_inntekt</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>on</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>on</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>on</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>1, 2, 3, 4, 5</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2024-11-29</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>900000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>